<commit_message>
Added recursive iteration for n no. of attempts for getting chatbot response
</commit_message>
<xml_diff>
--- a/response_with_status_temp.xlsx
+++ b/response_with_status_temp.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="status_sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -487,10 +487,10 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C13"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.0546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.07421875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="67.52" customWidth="1" style="3" min="1" max="1"/>
     <col width="40.29" customWidth="1" style="3" min="2" max="2"/>
@@ -552,7 +552,11 @@
           <t>Sorry I am busy</t>
         </is>
       </c>
-      <c r="C5" s="3" t="inlineStr"/>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>Rescheduled</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="4">
       <c r="A6" s="3" t="inlineStr"/>
@@ -615,11 +619,7 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="C12" s="3" t="inlineStr">
-        <is>
-          <t>Server Timeout</t>
-        </is>
-      </c>
+      <c r="C12" s="3" t="inlineStr"/>
     </row>
     <row r="13" ht="15" customHeight="1" s="4">
       <c r="A13" s="3" t="inlineStr"/>
@@ -657,10 +657,10 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C13"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.0546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.07421875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="98.37" customWidth="1" style="3" min="1" max="1"/>
     <col width="42.79" customWidth="1" style="3" min="2" max="2"/>
@@ -797,11 +797,11 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C13"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.0546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.07421875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="62.24" customWidth="1" style="3" min="1" max="1"/>
     <col width="25.98" customWidth="1" style="3" min="2" max="2"/>
@@ -955,10 +955,10 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C13"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.0546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.07421875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="47.82" customWidth="1" style="3" min="1" max="1"/>
     <col width="18.2" customWidth="1" style="3" min="2" max="2"/>
@@ -1111,11 +1111,11 @@
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C13"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.0546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.07421875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="45.98" customWidth="1" style="3" min="1" max="1"/>
     <col width="22.92" customWidth="1" style="3" min="2" max="2"/>
@@ -1253,10 +1253,10 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C13"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.0546875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.07421875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="55.85" customWidth="1" style="3" min="1" max="1"/>
     <col width="42.21" customWidth="1" style="3" min="2" max="2"/>

</xml_diff>